<commit_message>
Modified to pass first test.
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph_output.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph_output.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr date1904="1"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="160" yWindow="60" windowWidth="25600" windowHeight="16000" tabRatio="644" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -26,12 +26,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">network!$A$1:$V$22</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="39">
   <si>
     <t>CIN5</t>
   </si>
@@ -45,33 +50,12 @@
     <t>kk_max</t>
   </si>
   <si>
-    <t>SystematicName</t>
-  </si>
-  <si>
-    <t>StandardName</t>
-  </si>
-  <si>
-    <t>DegradationRate</t>
-  </si>
-  <si>
-    <t>YOR028C</t>
-  </si>
-  <si>
-    <t>YPR104C</t>
-  </si>
-  <si>
-    <t>rows genes affected/cols genes controlling</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
     <t>optimization_parameter</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>MaxIter</t>
   </si>
   <si>
@@ -84,21 +68,12 @@
     <t>TolX</t>
   </si>
   <si>
-    <t>YLR131C</t>
-  </si>
-  <si>
     <t>ACE2</t>
   </si>
   <si>
-    <t>production_rates</t>
-  </si>
-  <si>
     <t>AFT2</t>
   </si>
   <si>
-    <t>YPL202C</t>
-  </si>
-  <si>
     <t>Strain</t>
   </si>
   <si>
@@ -123,18 +98,6 @@
     <t>dcin5</t>
   </si>
   <si>
-    <t>simtime</t>
-  </si>
-  <si>
-    <t>estimateParams</t>
-  </si>
-  <si>
-    <t>makeGraphs</t>
-  </si>
-  <si>
-    <t>prorate</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -163,13 +126,40 @@
   </si>
   <si>
     <t>dcin5 SSE</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>production_rate</t>
+  </si>
+  <si>
+    <t>degradation_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulators/controllers </t>
+  </si>
+  <si>
+    <t>make_graphs</t>
+  </si>
+  <si>
+    <t>estimate_params</t>
+  </si>
+  <si>
+    <t>simulation_timepoints</t>
+  </si>
+  <si>
+    <t>expression_timepoints</t>
+  </si>
+  <si>
+    <t>threshold_b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -194,6 +184,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -212,9 +214,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -223,7 +227,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -240,8 +243,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -645,426 +651,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="13">
       <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
-      <c r="H1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" ht="13">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="B2">
         <v>0.5</v>
       </c>
-      <c r="H2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7" ht="13">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7" ht="13">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D4" s="5"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" ht="13">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7" ht="13">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="4"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7" ht="13">
       <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="4"/>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7" ht="13">
       <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="4"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" ht="13">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="4"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7" ht="13">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="4"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7" ht="13">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" s="4"/>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7" ht="13">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="4"/>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7" ht="13">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" ht="13">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="4"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" ht="13">
       <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15" s="4"/>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" ht="13">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="4"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" ht="13">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17" s="4"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" ht="13">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" s="4"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" ht="13">
       <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" ht="13">
       <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20" s="4"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" ht="13">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" ht="13">
       <c r="A22"/>
       <c r="B22"/>
-      <c r="C22"/>
-      <c r="H22"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E24" s="5"/>
+      <c r="G22"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="D24" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:W5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F1">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H1">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I1">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="J1">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="K1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="L1">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M1">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N1">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="O1">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="P1">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="Q1">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="R1">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="S1">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="T1">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="U1">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V1">
-        <v>1.9</v>
-      </c>
-      <c r="W1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-8.9800321449215181E-2</v>
       </c>
       <c r="D2">
-        <v>-8.9800321449215181E-2</v>
+        <v>-0.17783723566962159</v>
       </c>
       <c r="E2">
-        <v>-0.17783723566962159</v>
+        <v>-0.26414317546565297</v>
       </c>
       <c r="F2">
-        <v>-0.26414317546565297</v>
+        <v>-0.34875359461636379</v>
       </c>
       <c r="G2">
-        <v>-0.34875359461636379</v>
+        <v>-0.43170548228292405</v>
       </c>
       <c r="H2">
-        <v>-0.43170548228292405</v>
+        <v>-0.51303803932179959</v>
       </c>
       <c r="I2">
-        <v>-0.51303803932179959</v>
+        <v>-0.59279132706349291</v>
       </c>
       <c r="J2">
-        <v>-0.59279132706349291</v>
+        <v>-0.67100682676036338</v>
       </c>
       <c r="K2">
-        <v>-0.67100682676036338</v>
+        <v>-0.74772630271945129</v>
       </c>
       <c r="L2">
-        <v>-0.74772630271945129</v>
+        <v>-0.82299227598659463</v>
       </c>
       <c r="M2">
-        <v>-0.82299227598659463</v>
+        <v>-0.89684708166550642</v>
       </c>
       <c r="N2">
-        <v>-0.89684708166550642</v>
+        <v>-0.9693332787484078</v>
       </c>
       <c r="O2">
-        <v>-0.9693332787484078</v>
+        <v>-1.0404928780646217</v>
       </c>
       <c r="P2">
-        <v>-1.0404928780646217</v>
+        <v>-1.1103677031390775</v>
       </c>
       <c r="Q2">
-        <v>-1.1103677031390775</v>
+        <v>-1.1789987643329474</v>
       </c>
       <c r="R2">
-        <v>-1.1789987643329474</v>
+        <v>-1.2464265806106019</v>
       </c>
       <c r="S2">
-        <v>-1.2464265806106019</v>
+        <v>-1.3126906763676192</v>
       </c>
       <c r="T2">
-        <v>-1.3126906763676192</v>
+        <v>-1.377829870641254</v>
       </c>
       <c r="U2">
-        <v>-1.377829870641254</v>
+        <v>-1.4418818751815392</v>
       </c>
       <c r="V2">
-        <v>-1.4418818751815392</v>
-      </c>
-      <c r="W2">
         <v>-1.5048835406461176</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-5.3554472545191481E-2</v>
       </c>
       <c r="D3">
-        <v>-5.3554472545191481E-2</v>
+        <v>-0.10534033101746187</v>
       </c>
       <c r="E3">
-        <v>-0.10534033101746187</v>
+        <v>-0.15541295136192257</v>
       </c>
       <c r="F3">
-        <v>-0.15541295136192257</v>
+        <v>-0.2038273200147003</v>
       </c>
       <c r="G3">
-        <v>-0.2038273200147003</v>
+        <v>-0.25063751475470381</v>
       </c>
       <c r="H3">
-        <v>-0.25063751475470381</v>
+        <v>-0.29589686364454737</v>
       </c>
       <c r="I3">
-        <v>-0.29589686364454737</v>
+        <v>-0.33965752021893808</v>
       </c>
       <c r="J3">
-        <v>-0.33965752021893808</v>
+        <v>-0.38197061557552464</v>
       </c>
       <c r="K3">
-        <v>-0.38197061557552464</v>
+        <v>-0.42288593483478537</v>
       </c>
       <c r="L3">
-        <v>-0.42288593483478537</v>
+        <v>-0.46245206329717115</v>
       </c>
       <c r="M3">
-        <v>-0.46245206329717115</v>
+        <v>-0.5007161439761052</v>
       </c>
       <c r="N3">
-        <v>-0.5007161439761052</v>
+        <v>-0.53772401759212052</v>
       </c>
       <c r="O3">
-        <v>-0.53772401759212052</v>
+        <v>-0.57352004400459444</v>
       </c>
       <c r="P3">
-        <v>-0.57352004400459444</v>
+        <v>-0.60814723537794035</v>
       </c>
       <c r="Q3">
-        <v>-0.60814723537794035</v>
+        <v>-0.64164712729223439</v>
       </c>
       <c r="R3">
-        <v>-0.64164712729223439</v>
+        <v>-0.6740599043814397</v>
       </c>
       <c r="S3">
-        <v>-0.6740599043814397</v>
+        <v>-0.70542430959397973</v>
       </c>
       <c r="T3">
-        <v>-0.70542430959397973</v>
+        <v>-0.73577776176435217</v>
       </c>
       <c r="U3">
-        <v>-0.73577776176435217</v>
+        <v>-0.76515629383282446</v>
       </c>
       <c r="V3">
-        <v>-0.76515629383282446</v>
-      </c>
-      <c r="W3">
         <v>-0.79359465825360598</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
@@ -1127,145 +1096,138 @@
       <c r="V4">
         <v>0</v>
       </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-4.5851325928348091E-2</v>
       </c>
       <c r="D5">
-        <v>-4.5851325928348091E-2</v>
+        <v>-9.0834146060417342E-2</v>
       </c>
       <c r="E5">
-        <v>-9.0834146060417342E-2</v>
+        <v>-0.13497660518656263</v>
       </c>
       <c r="F5">
-        <v>-0.13497660518656263</v>
+        <v>-0.17830584843860664</v>
       </c>
       <c r="G5">
-        <v>-0.17830584843860664</v>
+        <v>-0.22084797637772191</v>
       </c>
       <c r="H5">
-        <v>-0.22084797637772191</v>
+        <v>-0.2626281490883578</v>
       </c>
       <c r="I5">
-        <v>-0.2626281490883578</v>
+        <v>-0.30367054964856338</v>
       </c>
       <c r="J5">
-        <v>-0.30367054964856338</v>
+        <v>-0.34399847763154839</v>
       </c>
       <c r="K5">
-        <v>-0.34399847763154839</v>
+        <v>-0.38363432380541679</v>
       </c>
       <c r="L5">
-        <v>-0.38363432380541679</v>
+        <v>-0.42259965397966681</v>
       </c>
       <c r="M5">
-        <v>-0.42259965397966681</v>
+        <v>-0.46091519214766763</v>
       </c>
       <c r="N5">
-        <v>-0.46091519214766763</v>
+        <v>-0.49860089557940129</v>
       </c>
       <c r="O5">
-        <v>-0.49860089557940129</v>
+        <v>-0.53567594426493337</v>
       </c>
       <c r="P5">
-        <v>-0.53567594426493337</v>
+        <v>-0.57215880810708175</v>
       </c>
       <c r="Q5">
-        <v>-0.57215880810708175</v>
+        <v>-0.60806724102672904</v>
       </c>
       <c r="R5">
-        <v>-0.60806724102672904</v>
+        <v>-0.64341834105334972</v>
       </c>
       <c r="S5">
-        <v>-0.64341834105334972</v>
+        <v>-0.678228547842608</v>
       </c>
       <c r="T5">
-        <v>-0.678228547842608</v>
+        <v>-0.71251369640221618</v>
       </c>
       <c r="U5">
-        <v>-0.71251369640221618</v>
+        <v>-0.74628901707297057</v>
       </c>
       <c r="V5">
-        <v>-0.74628901707297057</v>
-      </c>
-      <c r="W5">
         <v>-0.77956918237391504</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>0.4</v>
       </c>
       <c r="C1">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D1">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="E1">
-        <v>1.2</v>
-      </c>
-      <c r="F1">
         <v>1.6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>6.7986997775525911E-17</v>
       </c>
       <c r="C2">
-        <v>6.7986997775525911E-17</v>
+        <v>1.3597399555105182E-16</v>
       </c>
       <c r="D2">
-        <v>1.3597399555105182E-16</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>3.3993498887762956E-17</v>
       </c>
       <c r="C3">
-        <v>3.3993498887762956E-17</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1273,15 +1235,12 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
@@ -1293,16 +1252,13 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1311,76 +1267,72 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>0.4</v>
       </c>
       <c r="C1">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D1">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="E1">
-        <v>1.2</v>
-      </c>
-      <c r="F1">
         <v>1.6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>6.7986997775525911E-17</v>
       </c>
       <c r="C2">
-        <v>6.7986997775525911E-17</v>
+        <v>1.3597399555105182E-16</v>
       </c>
       <c r="D2">
-        <v>1.3597399555105182E-16</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>3.3993498887762956E-17</v>
       </c>
       <c r="C3">
-        <v>3.3993498887762956E-17</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1388,15 +1340,12 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
@@ -1408,16 +1357,13 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1426,84 +1372,76 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="B2">
         <v>0.69740719366499726</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="B3">
         <v>1.1568003225019745</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>2.7591362546192006</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>2.3785237031173372</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1511,21 +1449,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1534,9 +1470,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1.1390375115164613</v>
@@ -1551,9 +1487,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1568,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1521,7 @@
         <v>1.3472374603129511</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1604,6 +1540,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1615,67 +1556,67 @@
       <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>5.6205951121146291E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>2.1248299830536412</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>1.2133358649639586E-33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>1012</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>8.9376526217303694E-3</v>
@@ -1684,9 +1625,9 @@
         <v>1.7875305243460739E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>5.5824917406711817E-3</v>
@@ -1695,7 +1636,7 @@
         <v>1.1164983481342363E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1706,7 +1647,7 @@
         <v>3.9542102024695807E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1719,189 +1660,166 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="13">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" ht="13">
       <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="13">
       <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" ht="13">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" ht="13">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" ht="13">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" ht="13">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" ht="13">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" ht="13">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="13">
       <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2" ht="13">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" ht="13">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" ht="13">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" ht="13">
       <c r="A19"/>
       <c r="B19"/>
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" ht="13">
       <c r="A20"/>
       <c r="B20"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" ht="13">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" ht="13">
       <c r="A22"/>
       <c r="B22"/>
-      <c r="C22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="B1" s="10">
+        <v>0.4</v>
       </c>
       <c r="C1" s="11">
         <v>0.4</v>
@@ -1910,7 +1828,7 @@
         <v>0.4</v>
       </c>
       <c r="E1" s="13">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="F1" s="14">
         <v>0.8</v>
@@ -1919,16 +1837,16 @@
         <v>0.8</v>
       </c>
       <c r="H1" s="16">
-        <v>0.8</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="I1" s="17">
         <v>1.2000000000000002</v>
       </c>
       <c r="J1" s="18">
-        <v>1.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="K1" s="19">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="L1" s="20">
         <v>1.6</v>
@@ -1936,17 +1854,14 @@
       <c r="M1" s="21">
         <v>1.6</v>
       </c>
-      <c r="N1" s="22">
-        <v>1.6</v>
-      </c>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="14">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="10">
+        <v>-0.37633430629205178</v>
       </c>
       <c r="C2" s="11">
         <v>-0.37633430629205178</v>
@@ -1955,7 +1870,7 @@
         <v>-0.37633430629205178</v>
       </c>
       <c r="E2" s="13">
-        <v>-0.37633430629205178</v>
+        <v>-0.70666646734338179</v>
       </c>
       <c r="F2" s="14">
         <v>-0.70666646734338179</v>
@@ -1964,7 +1879,7 @@
         <v>-0.70666646734338179</v>
       </c>
       <c r="H2" s="16">
-        <v>-0.70666646734338179</v>
+        <v>-0.98723929967009216</v>
       </c>
       <c r="I2" s="17">
         <v>-0.98723929967009216</v>
@@ -1973,7 +1888,7 @@
         <v>-0.98723929967009216</v>
       </c>
       <c r="K2" s="19">
-        <v>-0.98723929967009216</v>
+        <v>-1.2174432654761544</v>
       </c>
       <c r="L2" s="20">
         <v>-1.2174432654761544</v>
@@ -1981,16 +1896,13 @@
       <c r="M2" s="21">
         <v>-1.2174432654761544</v>
       </c>
-      <c r="N2" s="22">
-        <v>-1.2174432654761544</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" ht="14">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="10">
+        <v>-0.22771865423983556</v>
       </c>
       <c r="C3" s="11">
         <v>-0.22771865423983556</v>
@@ -1999,7 +1911,7 @@
         <v>-0.22771865423983556</v>
       </c>
       <c r="E3" s="13">
-        <v>-0.22771865423983556</v>
+        <v>-0.40801774302656463</v>
       </c>
       <c r="F3" s="14">
         <v>-0.40801774302656463</v>
@@ -2008,7 +1920,7 @@
         <v>-0.40801774302656463</v>
       </c>
       <c r="H3" s="16">
-        <v>-0.40801774302656463</v>
+        <v>-0.5464126532391167</v>
       </c>
       <c r="I3" s="17">
         <v>-0.5464126532391167</v>
@@ -2017,7 +1929,7 @@
         <v>-0.5464126532391167</v>
       </c>
       <c r="K3" s="19">
-        <v>-0.5464126532391167</v>
+        <v>-0.64984386018298912</v>
       </c>
       <c r="L3" s="20">
         <v>-0.64984386018298912</v>
@@ -2025,16 +1937,13 @@
       <c r="M3" s="21">
         <v>-0.64984386018298912</v>
       </c>
-      <c r="N3" s="22">
-        <v>-0.64984386018298912</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" ht="14">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.26929382132237512</v>
       </c>
       <c r="C4" s="11">
         <v>0.26929382132237512</v>
@@ -2043,7 +1952,7 @@
         <v>0.26929382132237512</v>
       </c>
       <c r="E4" s="13">
-        <v>0.26929382132237512</v>
+        <v>0.41593537248224854</v>
       </c>
       <c r="F4" s="14">
         <v>0.41593537248224854</v>
@@ -2052,7 +1961,7 @@
         <v>0.41593537248224854</v>
       </c>
       <c r="H4" s="16">
-        <v>0.41593537248224854</v>
+        <v>0.49751163358969142</v>
       </c>
       <c r="I4" s="17">
         <v>0.49751163358969142</v>
@@ -2061,7 +1970,7 @@
         <v>0.49751163358969142</v>
       </c>
       <c r="K4" s="19">
-        <v>0.49751163358969142</v>
+        <v>0.54159993841241572</v>
       </c>
       <c r="L4" s="20">
         <v>0.54159993841241572</v>
@@ -2069,16 +1978,13 @@
       <c r="M4" s="21">
         <v>0.54159993841241572</v>
       </c>
-      <c r="N4" s="22">
-        <v>0.54159993841241572</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" ht="14">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="10">
+        <v>-0.29093615522070321</v>
       </c>
       <c r="C5" s="11">
         <v>-0.29093615522070321</v>
@@ -2087,7 +1993,7 @@
         <v>-0.29093615522070321</v>
       </c>
       <c r="E5" s="13">
-        <v>-0.29093615522070321</v>
+        <v>-0.57977180156386388</v>
       </c>
       <c r="F5" s="14">
         <v>-0.57977180156386388</v>
@@ -2096,7 +2002,7 @@
         <v>-0.57977180156386388</v>
       </c>
       <c r="H5" s="16">
-        <v>-0.57977180156386388</v>
+        <v>-0.85583465653557034</v>
       </c>
       <c r="I5" s="17">
         <v>-0.85583465653557034</v>
@@ -2105,7 +2011,7 @@
         <v>-0.85583465653557034</v>
       </c>
       <c r="K5" s="19">
-        <v>-0.85583465653557034</v>
+        <v>-1.1097262320569594</v>
       </c>
       <c r="L5" s="20">
         <v>-1.1097262320569594</v>
@@ -2113,329 +2019,321 @@
       <c r="M5" s="21">
         <v>-1.1097262320569594</v>
       </c>
-      <c r="N5" s="22">
-        <v>-1.1097262320569594</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G6" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G12" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I14" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="I18" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="B16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="H18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="F20" s="2"/>
-      <c r="M20" s="2"/>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:12">
+      <c r="E20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="10">
+        <v>30</v>
+      </c>
+      <c r="B1" s="9">
         <v>0.4</v>
       </c>
-      <c r="D1" s="10">
+      <c r="C1" s="9">
         <v>0.4</v>
       </c>
-      <c r="E1" s="10">
+      <c r="D1" s="9">
         <v>0.4</v>
       </c>
-      <c r="F1" s="10">
+      <c r="E1" s="9">
         <v>0.8</v>
       </c>
-      <c r="G1" s="10">
+      <c r="F1" s="9">
         <v>0.8</v>
       </c>
-      <c r="H1" s="10">
+      <c r="G1" s="9">
         <v>0.8</v>
       </c>
-      <c r="I1" s="10">
+      <c r="H1" s="9">
         <v>1.2000000000000002</v>
       </c>
-      <c r="J1" s="10">
+      <c r="I1" s="9">
         <v>1.2000000000000002</v>
       </c>
-      <c r="K1" s="10">
+      <c r="J1" s="9">
         <v>1.2</v>
       </c>
-      <c r="L1" s="10">
+      <c r="K1" s="9">
         <v>1.6</v>
       </c>
-      <c r="M1" s="10">
+      <c r="L1" s="9">
         <v>1.6</v>
       </c>
-      <c r="N1" s="10">
+      <c r="M1" s="9">
         <v>1.6</v>
       </c>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="14">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="10">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="D2" s="10">
+      <c r="C2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="E2" s="10">
+      <c r="D2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="F2" s="10">
+      <c r="E2" s="9">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="G2" s="10">
+      <c r="F2" s="9">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="H2" s="10">
+      <c r="G2" s="9">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="I2" s="10">
+      <c r="H2" s="9">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="J2" s="10">
+      <c r="I2" s="9">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="K2" s="10">
+      <c r="J2" s="9">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="L2" s="10">
+      <c r="K2" s="9">
         <v>-1.2174432654761544</v>
       </c>
-      <c r="M2" s="10">
+      <c r="L2" s="9">
         <v>-1.2174432654761544</v>
       </c>
-      <c r="N2" s="10">
+      <c r="M2" s="9">
         <v>-1.2174432654761544</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="14">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="10">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="D3" s="10">
+      <c r="C3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="E3" s="10">
+      <c r="D3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="F3" s="10">
+      <c r="E3" s="9">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="G3" s="10">
+      <c r="F3" s="9">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="H3" s="10">
+      <c r="G3" s="9">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="I3" s="10">
+      <c r="H3" s="9">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="J3" s="10">
+      <c r="I3" s="9">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="K3" s="10">
+      <c r="J3" s="9">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="L3" s="10">
+      <c r="K3" s="9">
         <v>-0.64984386018298912</v>
       </c>
-      <c r="M3" s="10">
+      <c r="L3" s="9">
         <v>-0.64984386018298912</v>
       </c>
-      <c r="N3" s="10">
+      <c r="M3" s="9">
         <v>-0.64984386018298912</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="14">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-      <c r="I4" s="10">
-        <v>0</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0</v>
-      </c>
-      <c r="M4" s="10">
-        <v>0</v>
-      </c>
-      <c r="N4" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="14">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="D5" s="10">
+      <c r="C5" s="9">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="E5" s="10">
+      <c r="D5" s="9">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="F5" s="10">
+      <c r="E5" s="9">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="G5" s="10">
+      <c r="F5" s="9">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="H5" s="10">
+      <c r="G5" s="9">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="I5" s="10">
+      <c r="H5" s="9">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="J5" s="10">
+      <c r="I5" s="9">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="K5" s="10">
+      <c r="J5" s="9">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="L5" s="10">
+      <c r="K5" s="9">
         <v>-0.40259011361710589</v>
       </c>
-      <c r="M5" s="10">
+      <c r="L5" s="9">
         <v>-0.40259011361710589</v>
       </c>
-      <c r="N5" s="10">
+      <c r="M5" s="9">
         <v>-0.40259011361710589</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="L7" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
+      <c r="B6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="18" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="I19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="I20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="22" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="L22" s="2"/>
-      <c r="N22" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="E11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="E13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="18" spans="6:13">
+      <c r="F18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="6:13">
+      <c r="H19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="6:13">
+      <c r="H20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="22" spans="6:13">
+      <c r="K22" s="2"/>
+      <c r="M22" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2443,41 +2341,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
+    <row r="1" spans="1:5">
+      <c r="A1" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -2486,9 +2382,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2503,9 +2399,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -2520,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -2537,7 +2433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -2559,6 +2455,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2566,40 +2467,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
+    <row r="1" spans="1:22">
+      <c r="A1" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2625,9 +2524,9 @@
       <c r="U1"/>
       <c r="V1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2642,9 +2541,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -2659,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2676,7 +2575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2698,6 +2597,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2706,35 +2610,35 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2742,7 +2646,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2750,83 +2654,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="12.75" customHeight="1">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="9">
+        <v>37</v>
+      </c>
+      <c r="B13" s="8">
         <v>0.4</v>
       </c>
       <c r="C13">
@@ -2839,42 +2743,42 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="8">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7">
         <v>3</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="8">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7">
         <v>0</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2945,6 +2849,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2952,34 +2861,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2987,7 +2899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2995,384 +2907,379 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:W5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F1">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H1">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I1">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="J1">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="K1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="L1">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M1">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N1">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="O1">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="P1">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="Q1">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="R1">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="S1">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="T1">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="U1">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V1">
-        <v>1.9</v>
-      </c>
-      <c r="W1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-8.9800321449215181E-2</v>
       </c>
       <c r="D2">
-        <v>-8.9800321449215181E-2</v>
+        <v>-0.17783723566962159</v>
       </c>
       <c r="E2">
-        <v>-0.17783723566962159</v>
+        <v>-0.26414317546565297</v>
       </c>
       <c r="F2">
-        <v>-0.26414317546565297</v>
+        <v>-0.34875359461636379</v>
       </c>
       <c r="G2">
-        <v>-0.34875359461636379</v>
+        <v>-0.43170548228292405</v>
       </c>
       <c r="H2">
-        <v>-0.43170548228292405</v>
+        <v>-0.51303803932179959</v>
       </c>
       <c r="I2">
-        <v>-0.51303803932179959</v>
+        <v>-0.59279132706349291</v>
       </c>
       <c r="J2">
-        <v>-0.59279132706349291</v>
+        <v>-0.67100682676036338</v>
       </c>
       <c r="K2">
-        <v>-0.67100682676036338</v>
+        <v>-0.74772630271945129</v>
       </c>
       <c r="L2">
-        <v>-0.74772630271945129</v>
+        <v>-0.82299227598659463</v>
       </c>
       <c r="M2">
-        <v>-0.82299227598659463</v>
+        <v>-0.89684708166550642</v>
       </c>
       <c r="N2">
-        <v>-0.89684708166550642</v>
+        <v>-0.9693332787484078</v>
       </c>
       <c r="O2">
-        <v>-0.9693332787484078</v>
+        <v>-1.0404928780646217</v>
       </c>
       <c r="P2">
-        <v>-1.0404928780646217</v>
+        <v>-1.1103677031390775</v>
       </c>
       <c r="Q2">
-        <v>-1.1103677031390775</v>
+        <v>-1.1789987643329474</v>
       </c>
       <c r="R2">
-        <v>-1.1789987643329474</v>
+        <v>-1.2464265806106019</v>
       </c>
       <c r="S2">
-        <v>-1.2464265806106019</v>
+        <v>-1.3126906763676192</v>
       </c>
       <c r="T2">
-        <v>-1.3126906763676192</v>
+        <v>-1.377829870641254</v>
       </c>
       <c r="U2">
-        <v>-1.377829870641254</v>
+        <v>-1.4418818751815392</v>
       </c>
       <c r="V2">
-        <v>-1.4418818751815392</v>
-      </c>
-      <c r="W2">
         <v>-1.5048835406461176</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-5.3554472545191481E-2</v>
       </c>
       <c r="D3">
-        <v>-5.3554472545191481E-2</v>
+        <v>-0.10534033101746187</v>
       </c>
       <c r="E3">
-        <v>-0.10534033101746187</v>
+        <v>-0.15541295136192257</v>
       </c>
       <c r="F3">
-        <v>-0.15541295136192257</v>
+        <v>-0.2038273200147003</v>
       </c>
       <c r="G3">
-        <v>-0.2038273200147003</v>
+        <v>-0.25063751475470381</v>
       </c>
       <c r="H3">
-        <v>-0.25063751475470381</v>
+        <v>-0.29589686364454737</v>
       </c>
       <c r="I3">
-        <v>-0.29589686364454737</v>
+        <v>-0.33965752021893808</v>
       </c>
       <c r="J3">
-        <v>-0.33965752021893808</v>
+        <v>-0.38197061557552464</v>
       </c>
       <c r="K3">
-        <v>-0.38197061557552464</v>
+        <v>-0.42288593483478537</v>
       </c>
       <c r="L3">
-        <v>-0.42288593483478537</v>
+        <v>-0.46245206329717115</v>
       </c>
       <c r="M3">
-        <v>-0.46245206329717115</v>
+        <v>-0.5007161439761052</v>
       </c>
       <c r="N3">
-        <v>-0.5007161439761052</v>
+        <v>-0.53772401759212052</v>
       </c>
       <c r="O3">
-        <v>-0.53772401759212052</v>
+        <v>-0.57352004400459444</v>
       </c>
       <c r="P3">
-        <v>-0.57352004400459444</v>
+        <v>-0.60814723537794035</v>
       </c>
       <c r="Q3">
-        <v>-0.60814723537794035</v>
+        <v>-0.64164712729223439</v>
       </c>
       <c r="R3">
-        <v>-0.64164712729223439</v>
+        <v>-0.6740599043814397</v>
       </c>
       <c r="S3">
-        <v>-0.6740599043814397</v>
+        <v>-0.70542430959397973</v>
       </c>
       <c r="T3">
-        <v>-0.70542430959397973</v>
+        <v>-0.73577776176435217</v>
       </c>
       <c r="U3">
-        <v>-0.73577776176435217</v>
+        <v>-0.76515629383282446</v>
       </c>
       <c r="V3">
-        <v>-0.76515629383282446</v>
-      </c>
-      <c r="W3">
         <v>-0.79359465825360598</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>7.4345920314281444E-2</v>
       </c>
       <c r="D4">
-        <v>7.4345920314281444E-2</v>
+        <v>0.1387862873421718</v>
       </c>
       <c r="E4">
-        <v>0.1387862873421718</v>
+        <v>0.19504398075803131</v>
       </c>
       <c r="F4">
-        <v>0.19504398075803131</v>
+        <v>0.24445619535924734</v>
       </c>
       <c r="G4">
-        <v>0.24445619535924734</v>
+        <v>0.28808099282175181</v>
       </c>
       <c r="H4">
-        <v>0.28808099282175181</v>
+        <v>0.3267702767439874</v>
       </c>
       <c r="I4">
-        <v>0.3267702767439874</v>
+        <v>0.36121939459262042</v>
       </c>
       <c r="J4">
-        <v>0.36121939459262042</v>
+        <v>0.39200333574599211</v>
       </c>
       <c r="K4">
-        <v>0.39200333574599211</v>
+        <v>0.41960228361880236</v>
       </c>
       <c r="L4">
-        <v>0.41960228361880236</v>
+        <v>0.44442125188544235</v>
       </c>
       <c r="M4">
-        <v>0.44442125188544235</v>
+        <v>0.46680430214292035</v>
       </c>
       <c r="N4">
-        <v>0.46680430214292035</v>
+        <v>0.48704596892456742</v>
       </c>
       <c r="O4">
-        <v>0.48704596892456742</v>
+        <v>0.50539967340460468</v>
       </c>
       <c r="P4">
-        <v>0.50539967340460468</v>
+        <v>0.5220847587784978</v>
       </c>
       <c r="Q4">
-        <v>0.5220847587784978</v>
+        <v>0.53729173165300481</v>
       </c>
       <c r="R4">
-        <v>0.53729173165300481</v>
+        <v>0.55118680460021641</v>
       </c>
       <c r="S4">
-        <v>0.55118680460021641</v>
+        <v>0.56391531043720267</v>
       </c>
       <c r="T4">
-        <v>0.56391531043720267</v>
+        <v>0.57560475729047178</v>
       </c>
       <c r="U4">
-        <v>0.57560475729047178</v>
+        <v>0.58636714421203395</v>
       </c>
       <c r="V4">
-        <v>0.58636714421203395</v>
-      </c>
-      <c r="W4">
         <v>0.5963010868083789</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-5.8604556661095743E-2</v>
       </c>
       <c r="D5">
-        <v>-5.8604556661095743E-2</v>
+        <v>-0.11678083924349103</v>
       </c>
       <c r="E5">
-        <v>-0.11678083924349103</v>
+        <v>-0.17448802461226795</v>
       </c>
       <c r="F5">
-        <v>-0.17448802461226795</v>
+        <v>-0.23168628341320835</v>
       </c>
       <c r="G5">
-        <v>-0.23168628341320835</v>
+        <v>-0.28833618327924054</v>
       </c>
       <c r="H5">
-        <v>-0.28833618327924054</v>
+        <v>-0.34439836996876116</v>
       </c>
       <c r="I5">
-        <v>-0.34439836996876116</v>
+        <v>-0.39983318516774291</v>
       </c>
       <c r="J5">
-        <v>-0.39983318516774291</v>
+        <v>-0.45460058100867851</v>
       </c>
       <c r="K5">
-        <v>-0.45460058100867851</v>
+        <v>-0.50865989173411208</v>
       </c>
       <c r="L5">
-        <v>-0.50865989173411208</v>
+        <v>-0.56196992615853658</v>
       </c>
       <c r="M5">
-        <v>-0.56196992615853658</v>
+        <v>-0.61448886482108267</v>
       </c>
       <c r="N5">
-        <v>-0.61448886482108267</v>
+        <v>-0.66617449926014538</v>
       </c>
       <c r="O5">
-        <v>-0.66617449926014538</v>
+        <v>-0.71698423762054075</v>
       </c>
       <c r="P5">
-        <v>-0.71698423762054075</v>
+        <v>-0.76687546770195336</v>
       </c>
       <c r="Q5">
-        <v>-0.76687546770195336</v>
+        <v>-0.81580565499870039</v>
       </c>
       <c r="R5">
-        <v>-0.81580565499870039</v>
+        <v>-0.86373280603844371</v>
       </c>
       <c r="S5">
-        <v>-0.86373280603844371</v>
+        <v>-0.91061563837583892</v>
       </c>
       <c r="T5">
-        <v>-0.91061563837583892</v>
+        <v>-0.9564141159027354</v>
       </c>
       <c r="U5">
-        <v>-0.9564141159027354</v>
+        <v>-1.0010896635263178</v>
       </c>
       <c r="V5">
-        <v>-1.0010896635263178</v>
-      </c>
-      <c r="W5">
         <v>-1.0446057291203115</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed extra space :(
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph_output.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph_output.xlsx
@@ -137,9 +137,6 @@
     <t>degradation_rate</t>
   </si>
   <si>
-    <t xml:space="preserve">regulators/controllers </t>
-  </si>
-  <si>
     <t>make_graphs</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>threshold_b</t>
+  </si>
+  <si>
+    <t>regulators/controllers</t>
   </si>
 </sst>
 </file>
@@ -1455,7 +1455,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -2367,7 +2367,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="22" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -2492,7 +2492,7 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="22" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="8">
         <v>1</v>
@@ -2728,7 +2728,7 @@
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="8">
         <v>0.4</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2861,18 +2861,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
Update so that the SSE is now MSE in the optimization diagnostics sheet
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph_output.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph_output.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="165" yWindow="60" windowWidth="19440" windowHeight="15600" tabRatio="644" firstSheet="13" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -119,12 +119,6 @@
     <t>Gene</t>
   </si>
   <si>
-    <t>wt SSE</t>
-  </si>
-  <si>
-    <t>dcin5 SSE</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>production_function</t>
+  </si>
+  <si>
+    <t>wt MSE</t>
+  </si>
+  <si>
+    <t>dcin5 MSE</t>
   </si>
 </sst>
 </file>
@@ -675,10 +675,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -837,7 +837,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -1197,7 +1197,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1">
         <v>0.4</v>
@@ -1302,7 +1302,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1">
         <v>0.4</v>
@@ -1407,10 +1407,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1465,7 +1465,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1562,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1618,10 +1618,10 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1695,10 +1695,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1826,7 +1826,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="10">
         <v>0.4</v>
@@ -2083,7 +2083,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="9">
         <v>0.4</v>
@@ -2377,7 +2377,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -2502,7 +2502,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -2619,7 +2619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -2698,15 +2698,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="8">
         <v>1</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" s="8">
         <v>0.4</v>
@@ -2796,7 +2796,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2887,10 +2887,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2954,7 +2954,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1">
         <v>0</v>

</xml_diff>